<commit_message>
update dates for testing data
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -290,7 +290,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -336,13 +336,13 @@
         <v>8</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>45888</v>
+        <v>45980</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>45895</v>
+        <v>45987</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>4</v>

</xml_diff>